<commit_message>
Add another point for auto shot
</commit_message>
<xml_diff>
--- a/ShotTuner.xlsx
+++ b/ShotTuner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/roberthilton/repos/turret_node/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9002083E-60FF-AE45-98C7-8C8A7D145542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080B5482-85F0-A94B-8CE3-64312F75F80A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{A8A6C936-3468-D34A-A6E8-38D90E761E93}"/>
   </bookViews>
@@ -222,10 +222,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Shots!$A$2:$A$26</c:f>
+              <c:f>Shots!$A$2:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>1.161</c:v>
                 </c:pt>
@@ -275,30 +275,33 @@
                   <c:v>7.13</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>7.38</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>7.66</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>7.93</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>8.3699999999999992</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>8.99</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>9.19</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>9.4</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>10.065</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>10.26</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>10.8</c:v>
                 </c:pt>
               </c:numCache>
@@ -306,10 +309,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Shots!$B$2:$B$26</c:f>
+              <c:f>Shots!$B$2:$B$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>1207.375</c:v>
                 </c:pt>
@@ -356,33 +359,36 @@
                   <c:v>1750</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1800</c:v>
+                  <c:v>1835</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>1900</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1930</c:v>
+                  <c:v>1920</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>1940</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>1970</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>2025</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>2052.1759259259261</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>2075.3703703703704</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>2143.8194444444443</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>2217.5</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>2215</c:v>
                 </c:pt>
               </c:numCache>
@@ -697,10 +703,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Shots!$E$2:$E$26</c:f>
+              <c:f>Shots!$E$2:$E$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>1.161</c:v>
                 </c:pt>
@@ -749,31 +755,31 @@
                 <c:pt idx="15">
                   <c:v>7.13</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>7.66</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>7.93</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>8.3699999999999992</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>8.99</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>9.19</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>9.4</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>10.065</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>10.26</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>10.8</c:v>
                 </c:pt>
               </c:numCache>
@@ -781,10 +787,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Shots!$F$2:$F$26</c:f>
+              <c:f>Shots!$F$2:$F$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>1255</c:v>
                 </c:pt>
@@ -833,31 +839,31 @@
                 <c:pt idx="15">
                   <c:v>2080</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>2180</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>2240</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>2330</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>2430</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>2505</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>2530</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>2630</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>2730</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>2755</c:v>
                 </c:pt>
               </c:numCache>
@@ -2181,7 +2187,7 @@
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2546,10 +2552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7BD05DA-49E1-1044-A594-9EC79BFF86DC}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2576,7 +2582,7 @@
         <v>1207.375</v>
       </c>
       <c r="C2">
-        <f>B2-A2/$A$26*350</f>
+        <f>B2-A2/$A$27*350</f>
         <v>1169.75</v>
       </c>
       <c r="E2">
@@ -2594,7 +2600,7 @@
         <v>1197.2638888888889</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C26" si="0">B3-A3/$A$26*350</f>
+        <f t="shared" ref="C3:C27" si="0">B3-A3/$A$27*350</f>
         <v>1149.5277777777778</v>
       </c>
       <c r="E3">
@@ -2843,11 +2849,15 @@
         <v>7.13</v>
       </c>
       <c r="B17">
-        <v>1800</v>
+        <v>1835</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>1568.9351851851852</v>
+        <v>1603.9351851851852</v>
+      </c>
+      <c r="D17">
+        <f>FORECAST(7.43,B18:B19,A18:A19)</f>
+        <v>1903.5714285714287</v>
       </c>
       <c r="E17">
         <v>7.13</v>
@@ -2858,163 +2868,175 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>7.66</v>
+        <v>7.38</v>
       </c>
       <c r="B18">
         <v>1900</v>
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>1651.7592592592594</v>
-      </c>
-      <c r="E18">
-        <v>7.66</v>
-      </c>
-      <c r="F18">
-        <v>2180</v>
+        <v>1660.8333333333335</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>7.93</v>
+        <v>7.66</v>
       </c>
       <c r="B19">
-        <v>1930</v>
+        <v>1920</v>
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>1673.0092592592594</v>
+        <v>1671.7592592592594</v>
       </c>
       <c r="E19">
-        <v>7.93</v>
+        <v>7.66</v>
       </c>
       <c r="F19">
-        <v>2240</v>
+        <v>2180</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>8.3699999999999992</v>
+        <v>7.93</v>
       </c>
       <c r="B20">
-        <v>1970</v>
+        <v>1940</v>
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>1698.75</v>
+        <v>1683.0092592592594</v>
       </c>
       <c r="E20">
-        <v>8.3699999999999992</v>
+        <v>7.93</v>
       </c>
       <c r="F20">
-        <v>2330</v>
+        <v>2240</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>8.99</v>
+        <v>8.3699999999999992</v>
       </c>
       <c r="B21">
-        <v>2025</v>
+        <v>1970</v>
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>1733.6574074074074</v>
+        <v>1698.75</v>
       </c>
       <c r="E21">
-        <v>8.99</v>
+        <v>8.3699999999999992</v>
       </c>
       <c r="F21">
-        <v>2430</v>
+        <v>2330</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>9.19</v>
+        <v>8.99</v>
       </c>
       <c r="B22">
-        <v>2052.1759259259261</v>
+        <v>2025</v>
       </c>
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>1754.351851851852</v>
+        <v>1733.6574074074074</v>
       </c>
       <c r="E22">
-        <v>9.19</v>
+        <v>8.99</v>
       </c>
       <c r="F22">
-        <v>2505</v>
+        <v>2430</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>9.4</v>
+        <v>9.19</v>
       </c>
       <c r="B23">
-        <v>2075.3703703703704</v>
+        <v>2052.1759259259261</v>
       </c>
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>1770.7407407407409</v>
+        <v>1754.351851851852</v>
       </c>
       <c r="E23">
-        <v>9.4</v>
+        <v>9.19</v>
       </c>
       <c r="F23">
-        <v>2530</v>
+        <v>2505</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>10.065</v>
+        <v>9.4</v>
       </c>
       <c r="B24">
-        <v>2143.8194444444443</v>
+        <v>2075.3703703703704</v>
       </c>
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>1817.6388888888887</v>
+        <v>1770.7407407407409</v>
       </c>
       <c r="E24">
-        <v>10.065</v>
+        <v>9.4</v>
       </c>
       <c r="F24">
-        <v>2630</v>
+        <v>2530</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>10.26</v>
+        <v>10.065</v>
       </c>
       <c r="B25">
-        <v>2217.5</v>
+        <v>2143.8194444444443</v>
       </c>
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>1885</v>
+        <v>1817.6388888888887</v>
       </c>
       <c r="E25">
-        <v>10.26</v>
+        <v>10.065</v>
       </c>
       <c r="F25">
-        <v>2730</v>
+        <v>2630</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>10.8</v>
+        <v>10.26</v>
       </c>
       <c r="B26">
-        <v>2215</v>
+        <v>2217.5</v>
       </c>
       <c r="C26">
         <f t="shared" si="0"/>
+        <v>1885</v>
+      </c>
+      <c r="E26">
+        <v>10.26</v>
+      </c>
+      <c r="F26">
+        <v>2730</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>10.8</v>
+      </c>
+      <c r="B27">
+        <v>2215</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
         <v>1865</v>
       </c>
-      <c r="E26">
+      <c r="E27">
         <v>10.8</v>
       </c>
-      <c r="F26">
+      <c r="F27">
         <v>2755</v>
       </c>
     </row>
@@ -3166,10 +3188,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CE86F5E-32B1-214C-8E6E-9224A47FDCB0}">
-  <dimension ref="A1:A25"/>
+  <dimension ref="A1:A26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A1:A25"/>
+      <selection activeCell="A26" sqref="A1:A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3267,60 +3289,66 @@
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="str">
         <f>"shooter_rpm_lookup_table.insert("&amp;Shots!A17&amp;","&amp;Shots!B17&amp;");"</f>
-        <v>shooter_rpm_lookup_table.insert(7.13,1800);</v>
+        <v>shooter_rpm_lookup_table.insert(7.13,1835);</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="str">
         <f>"shooter_rpm_lookup_table.insert("&amp;Shots!A18&amp;","&amp;Shots!B18&amp;");"</f>
-        <v>shooter_rpm_lookup_table.insert(7.66,1900);</v>
+        <v>shooter_rpm_lookup_table.insert(7.38,1900);</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="str">
         <f>"shooter_rpm_lookup_table.insert("&amp;Shots!A19&amp;","&amp;Shots!B19&amp;");"</f>
-        <v>shooter_rpm_lookup_table.insert(7.93,1930);</v>
+        <v>shooter_rpm_lookup_table.insert(7.66,1920);</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="str">
         <f>"shooter_rpm_lookup_table.insert("&amp;Shots!A20&amp;","&amp;Shots!B20&amp;");"</f>
-        <v>shooter_rpm_lookup_table.insert(8.37,1970);</v>
+        <v>shooter_rpm_lookup_table.insert(7.93,1940);</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="str">
         <f>"shooter_rpm_lookup_table.insert("&amp;Shots!A21&amp;","&amp;Shots!B21&amp;");"</f>
-        <v>shooter_rpm_lookup_table.insert(8.99,2025);</v>
+        <v>shooter_rpm_lookup_table.insert(8.37,1970);</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="str">
         <f>"shooter_rpm_lookup_table.insert("&amp;Shots!A22&amp;","&amp;Shots!B22&amp;");"</f>
-        <v>shooter_rpm_lookup_table.insert(9.19,2052.17592592593);</v>
+        <v>shooter_rpm_lookup_table.insert(8.99,2025);</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="str">
         <f>"shooter_rpm_lookup_table.insert("&amp;Shots!A23&amp;","&amp;Shots!B23&amp;");"</f>
-        <v>shooter_rpm_lookup_table.insert(9.4,2075.37037037037);</v>
+        <v>shooter_rpm_lookup_table.insert(9.19,2052.17592592593);</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="str">
         <f>"shooter_rpm_lookup_table.insert("&amp;Shots!A24&amp;","&amp;Shots!B24&amp;");"</f>
-        <v>shooter_rpm_lookup_table.insert(10.065,2143.81944444444);</v>
+        <v>shooter_rpm_lookup_table.insert(9.4,2075.37037037037);</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="str">
         <f>"shooter_rpm_lookup_table.insert("&amp;Shots!A25&amp;","&amp;Shots!B25&amp;");"</f>
-        <v>shooter_rpm_lookup_table.insert(10.26,2217.5);</v>
+        <v>shooter_rpm_lookup_table.insert(10.065,2143.81944444444);</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="str">
         <f>"shooter_rpm_lookup_table.insert("&amp;Shots!A26&amp;","&amp;Shots!B26&amp;");"</f>
+        <v>shooter_rpm_lookup_table.insert(10.26,2217.5);</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="str">
+        <f>"shooter_rpm_lookup_table.insert("&amp;Shots!A27&amp;","&amp;Shots!B27&amp;");"</f>
         <v>shooter_rpm_lookup_table.insert(10.8,2215);</v>
       </c>
     </row>

</xml_diff>